<commit_message>
Updated abstract and introduction
</commit_message>
<xml_diff>
--- a/JSEP submission/data/4. results/Tokens.xlsx
+++ b/JSEP submission/data/4. results/Tokens.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="24576" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="23040" windowHeight="9744"/>
   </bookViews>
   <sheets>
     <sheet name="Tokens" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
   <si>
     <t>[CTokenBool]</t>
   </si>
@@ -296,6 +296,21 @@
   </si>
   <si>
     <t>While the \texttt{IF} and \texttt{CHOOSE} functions can be part of reference expressions, there were no formulas in the datasets using them as such.</t>
+  </si>
+  <si>
+    <t>Named ranges with Cell.mpla</t>
+  </si>
+  <si>
+    <t>Named ranges greek characters, ?</t>
+  </si>
+  <si>
+    <t>Formula with string containing '\'</t>
+  </si>
+  <si>
+    <t>Whitespace-only sheet name</t>
+  </si>
+  <si>
+    <t>Strange characters in struncured references</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K76"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,6 +1187,21 @@
     <col min="15" max="15" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D1">
+        <f>C2-D2</f>
+        <v>7541840</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>8577426</v>
+      </c>
+      <c r="D2">
+        <f>1035586</f>
+        <v>1035586</v>
+      </c>
+    </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>48</v>
@@ -1212,14 +1242,14 @@
         <v>8048520</v>
       </c>
       <c r="H4" s="4">
-        <f>G4/$G$3</f>
+        <f t="shared" ref="H4:H43" si="0">G4/$G$3</f>
         <v>0.93838744199728363</v>
       </c>
       <c r="I4" s="6">
         <v>187297690</v>
       </c>
       <c r="J4" s="4">
-        <f>I4/$I$3</f>
+        <f t="shared" ref="J4:J43" si="1">I4/$I$3</f>
         <v>0.9892392992934621</v>
       </c>
       <c r="K4" t="str">
@@ -1242,18 +1272,18 @@
         <v>7961614</v>
       </c>
       <c r="H5" s="4">
-        <f>G5/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.92825495813264569</v>
       </c>
       <c r="I5" s="6">
         <v>186125582</v>
       </c>
       <c r="J5" s="4">
-        <f>I5/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.98304864474445908</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K43" si="0">A5&amp;" &amp; \texttt{" &amp;C5&amp; "} &amp; " &amp;" &amp; "&amp;TEXT(G5,"#,###")&amp; " &amp; "&amp;TEXT(H5,"0.00%") &amp;" &amp; "&amp;IF(D5=1,"\textbf{","")&amp;TEXT(I5,"#,###")&amp;IF(D5=1,"}","")&amp; " &amp; "&amp;IF(E5=1,"\textbf{","")&amp;TEXT(J5,"0.00%") &amp;IF(E5=1,"}","")&amp; "\\"</f>
+        <f t="shared" ref="K5:K43" si="2">A5&amp;" &amp; \texttt{" &amp;C5&amp; "} &amp; " &amp;" &amp; "&amp;TEXT(G5,"#,###")&amp; " &amp; "&amp;TEXT(H5,"0.00%") &amp;" &amp; "&amp;IF(D5=1,"\textbf{","")&amp;TEXT(I5,"#,###")&amp;IF(D5=1,"}","")&amp; " &amp; "&amp;IF(E5=1,"\textbf{","")&amp;TEXT(J5,"0.00%") &amp;IF(E5=1,"}","")&amp; "\\"</f>
         <v>CELL &amp; \texttt{=A5} &amp;  &amp; 7,961,614 &amp; 92.83% &amp; 186,125,582 &amp; 98.30%\\</v>
       </c>
     </row>
@@ -1275,18 +1305,18 @@
         <v>7017678</v>
       </c>
       <c r="H6" s="4">
-        <f>G6/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.81820022900863931</v>
       </c>
       <c r="I6" s="6">
         <v>163982378</v>
       </c>
       <c r="J6" s="4">
-        <f>I6/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.86609617400618044</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{FunctionCall} &amp; \texttt{=SUM(A5:A22)} &amp;  &amp; 7,017,678 &amp; 81.82% &amp; 163,982,378 &amp; \textbf{86.61%}\\</v>
       </c>
     </row>
@@ -1308,18 +1338,18 @@
         <v>3294376</v>
       </c>
       <c r="H7" s="4">
-        <f>G7/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.38409559367650742</v>
       </c>
       <c r="I7" s="6">
         <v>91984979</v>
       </c>
       <c r="J7" s="4">
-        <f>I7/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.48583170551374033</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{BinOp} &amp; \texttt{=H10-H8} &amp;  &amp; 3,294,376 &amp; 38.41% &amp; 91,984,979 &amp; \textbf{48.58%}\\</v>
       </c>
     </row>
@@ -1341,18 +1371,18 @@
         <v>4271892</v>
       </c>
       <c r="H8" s="4">
-        <f>G8/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.49806545878853009</v>
       </c>
       <c r="I8" s="6">
         <v>80850975</v>
       </c>
       <c r="J8" s="4">
-        <f>I8/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.42702588513608053</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>EXCEL-FUNCTION &amp; \texttt{=SUM(A5:A22)} &amp;  &amp; 4,271,892 &amp; 49.81% &amp; 80,850,975 &amp; \textbf{42.70%}\\</v>
       </c>
     </row>
@@ -1374,18 +1404,18 @@
         <v>4537173</v>
       </c>
       <c r="H9" s="4">
-        <f>G9/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.5289949165025547</v>
       </c>
       <c r="I9" s="6">
         <v>80185313</v>
       </c>
       <c r="J9" s="4">
-        <f>I9/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.42351009692509789</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{Constant} &amp; \texttt{=A5+134} &amp;  &amp; 4,537,173 &amp; 52.90% &amp; 80,185,313 &amp; \textbf{42.35%}\\</v>
       </c>
     </row>
@@ -1407,18 +1437,18 @@
         <v>2473935</v>
       </c>
       <c r="H10" s="4">
-        <f>G10/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.28843930763886405</v>
       </c>
       <c r="I10" s="6">
         <v>67421408</v>
       </c>
       <c r="J10" s="4">
-        <f>I10/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.35609572337650625</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>NUMBER &amp; \texttt{=(B8/48)*15} &amp;  &amp; 2,473,935 &amp; 28.84% &amp; 67,421,408 &amp; \textbf{35.61%}\\</v>
       </c>
     </row>
@@ -1440,18 +1470,18 @@
         <v>2918585</v>
       </c>
       <c r="H11" s="4">
-        <f>G11/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.34028163095844233</v>
       </c>
       <c r="I11" s="6">
         <v>54019709</v>
       </c>
       <c r="J11" s="4">
-        <f>I11/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.28531275040923743</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{Prefix} &amp; \texttt{=Sheet1!B1} &amp;  &amp; 2,918,585 &amp; 34.03% &amp; 54,019,709 &amp; \textbf{28.53%}\\</v>
       </c>
     </row>
@@ -1473,18 +1503,18 @@
         <v>1509887</v>
       </c>
       <c r="H12" s="4">
-        <f>G12/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.17603969420899154</v>
       </c>
       <c r="I12" s="6">
         <v>46037124</v>
       </c>
       <c r="J12" s="4">
-        <f>I12/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.24315159619558696</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{Reference} ':' \synt{Reference} &amp; \texttt{=SUM(A5:A22)} &amp;  &amp; 1,509,887 &amp; 17.60% &amp; 46,037,124 &amp; \textbf{24.32%}\\</v>
       </c>
     </row>
@@ -1506,18 +1536,18 @@
         <v>1399182</v>
       </c>
       <c r="H13" s="4">
-        <f>G13/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.16313245390067282</v>
       </c>
       <c r="I13" s="6">
         <v>34963857</v>
       </c>
       <c r="J13" s="4">
-        <f>I13/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.1846665668929329</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{UnOpPrefix} &amp; \texttt{=+B11+1} &amp;  &amp; 1,399,182 &amp; 16.31% &amp; 34,963,857 &amp; \textbf{18.47%}\\</v>
       </c>
     </row>
@@ -1539,18 +1569,18 @@
         <v>722407</v>
       </c>
       <c r="H14" s="4">
-        <f>G14/$G$3</f>
+        <f t="shared" si="0"/>
         <v>8.4226374142194055E-2</v>
       </c>
       <c r="I14" s="6">
         <v>28592583</v>
       </c>
       <c r="J14" s="4">
-        <f>I14/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.15101578013007078</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{RefFunctionName} &amp; \texttt{=SUM(J9:INDEX(J9:J41,B43))} &amp;  &amp; 722,407 &amp; 8.42% &amp; 28,592,583 &amp; \textbf{15.10%}\\</v>
       </c>
     </row>
@@ -1572,18 +1602,18 @@
         <v>682713</v>
       </c>
       <c r="H15" s="4">
-        <f>G15/$G$3</f>
+        <f t="shared" si="0"/>
         <v>7.9598398921577079E-2</v>
       </c>
       <c r="I15" s="6">
         <v>27747635</v>
       </c>
       <c r="J15" s="4">
-        <f>I15/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.14655306749619146</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>REF-FUNCTION-COND &amp; \texttt{=IF(A1&lt;0,0,1)} &amp;  &amp; 682,713 &amp; 7.96% &amp; 27,747,635 &amp; \textbf{14.66%}\\</v>
       </c>
     </row>
@@ -1605,18 +1635,18 @@
         <v>2529561</v>
       </c>
       <c r="H16" s="4">
-        <f>G16/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.29492481551466493</v>
       </c>
       <c r="I16" s="6">
         <v>25350954</v>
       </c>
       <c r="J16" s="4">
-        <f>I16/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.13389465706374057</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>STRING &amp; \texttt{=IF(AD3&lt;0,buy,sell)} &amp;  &amp; 2,529,561 &amp; 29.49% &amp; 25,350,954 &amp; \textbf{13.39%}\\</v>
       </c>
     </row>
@@ -1635,18 +1665,18 @@
         <v>1271751</v>
       </c>
       <c r="H17" s="4">
-        <f>G17/$G$3</f>
+        <f t="shared" si="0"/>
         <v>0.14827510744180142</v>
       </c>
       <c r="I17" s="6">
         <v>20255725</v>
       </c>
       <c r="J17" s="4">
-        <f>I17/$I$3</f>
+        <f t="shared" si="1"/>
         <v>0.10698348284851278</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>SHEET &amp; \texttt{=Sheet1!B1} &amp;  &amp; 1,271,751 &amp; 14.83% &amp; 20,255,725 &amp; 10.70%\\</v>
       </c>
     </row>
@@ -1665,18 +1695,18 @@
         <v>204060</v>
       </c>
       <c r="H18" s="4">
-        <f>G18/$G$3</f>
+        <f t="shared" si="0"/>
         <v>2.3791621492394339E-2</v>
       </c>
       <c r="I18" s="6">
         <v>17442457</v>
       </c>
       <c r="J18" s="4">
-        <f>I18/$I$3</f>
+        <f t="shared" si="1"/>
         <v>9.2124809124107948E-2</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>BOOL &amp; \texttt{=IF(AND(R11=1,R14=TRUE),G19,0)} &amp;  &amp; 204,060 &amp; 2.38% &amp; 17,442,457 &amp; 9.21%\\</v>
       </c>
     </row>
@@ -1698,18 +1728,18 @@
         <v>755875</v>
       </c>
       <c r="H19" s="4">
-        <f>G19/$G$3</f>
+        <f t="shared" si="0"/>
         <v>8.8128451904163352E-2</v>
       </c>
       <c r="I19" s="6">
         <v>15759824</v>
       </c>
       <c r="J19" s="4">
-        <f>I19/$I$3</f>
+        <f t="shared" si="1"/>
         <v>8.3237744420383869E-2</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>FILE &amp; \texttt{=[11]Sheet1!C5} &amp;  &amp; 755,875 &amp; 8.81% &amp; 15,759,824 &amp; \textbf{8.32%}\\</v>
       </c>
     </row>
@@ -1728,18 +1758,18 @@
         <v>318600</v>
       </c>
       <c r="H20" s="4">
-        <f>G20/$G$3</f>
+        <f t="shared" si="0"/>
         <v>3.7145989451518362E-2</v>
       </c>
       <c r="I20" s="6">
         <v>10466380</v>
       </c>
       <c r="J20" s="4">
-        <f>I20/$I$3</f>
+        <f t="shared" si="1"/>
         <v>5.5279669585562456E-2</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>QUOTED-FILE-SHEET &amp; \texttt{=('[2]Detail I\&amp;E'!D62)/1000} &amp;  &amp; 318,600 &amp; 3.71% &amp; 10,466,380 &amp; 5.53%\\</v>
       </c>
     </row>
@@ -1761,18 +1791,18 @@
         <v>244153</v>
       </c>
       <c r="H21" s="4">
-        <f>G21/$G$3</f>
+        <f t="shared" si="0"/>
         <v>2.8466116643303712E-2</v>
       </c>
       <c r="I21" s="6">
         <v>7927994</v>
       </c>
       <c r="J21" s="4">
-        <f>I21/$I$3</f>
+        <f t="shared" si="1"/>
         <v>4.1872824108843902E-2</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>VERTICAL-RANGE &amp; \texttt{=COUNT(A:A)} &amp;  &amp; 244,153 &amp; 2.85% &amp; 7,927,994 &amp; \textbf{4.19%}\\</v>
       </c>
     </row>
@@ -1794,18 +1824,18 @@
         <v>206336</v>
       </c>
       <c r="H22" s="4">
-        <f>G22/$G$3</f>
+        <f t="shared" si="0"/>
         <v>2.4056983300277755E-2</v>
       </c>
       <c r="I22" s="6">
         <v>3389407</v>
       </c>
       <c r="J22" s="4">
-        <f>I22/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.7901633520949221E-2</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{NamedRange} &amp; \texttt{=SUM(freq)} &amp;  &amp; 206,336 &amp; 2.41% &amp; 3,389,407 &amp; \textbf{1.79%}\\</v>
       </c>
     </row>
@@ -1827,18 +1857,18 @@
         <v>49753</v>
       </c>
       <c r="H23" s="4">
-        <f>G23/$G$3</f>
+        <f t="shared" si="0"/>
         <v>5.8007671474619993E-3</v>
       </c>
       <c r="I23" s="6">
         <v>1967840</v>
       </c>
       <c r="J23" s="4">
-        <f>I23/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.0393425902485218E-2</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>REF-FUNCTION &amp; \texttt{=SUM(J9:INDEX(J9:J41,B43))} &amp;  &amp; 49,753 &amp; 0.58% &amp; 1,967,840 &amp; \textbf{1.04%}\\</v>
       </c>
     </row>
@@ -1863,18 +1893,18 @@
         <v>72552</v>
       </c>
       <c r="H24" s="4">
-        <f>G24/$G$3</f>
+        <f t="shared" si="0"/>
         <v>8.4589322871517891E-3</v>
       </c>
       <c r="I24" s="6">
         <v>1963284</v>
       </c>
       <c r="J24" s="4">
-        <f>I24/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.036936274266952E-2</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>UDF &amp; \texttt{=SQRT(_eoq2(C5,C4,C6,C7))} &amp;  &amp; 72,552 &amp; 0.85% &amp; \textbf{1,963,284} &amp; \textbf{1.04%}\\</v>
       </c>
     </row>
@@ -1896,18 +1926,18 @@
         <v>57375</v>
       </c>
       <c r="H25" s="4">
-        <f>G25/$G$3</f>
+        <f t="shared" si="0"/>
         <v>6.6894260664810612E-3</v>
       </c>
       <c r="I25" s="6">
         <v>1435260</v>
       </c>
       <c r="J25" s="4">
-        <f>I25/$I$3</f>
+        <f t="shared" si="1"/>
         <v>7.5805291389548606E-3</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ERROR-REF &amp; \texttt{=AVERAGE(#REF!)} &amp;  &amp; 57,375 &amp; 0.67% &amp; 1,435,260 &amp; \textbf{0.76%}\\</v>
       </c>
     </row>
@@ -1929,18 +1959,18 @@
         <v>50575</v>
       </c>
       <c r="H26" s="4">
-        <f>G26/$G$3</f>
+        <f t="shared" si="0"/>
         <v>5.8966051993425651E-3</v>
       </c>
       <c r="I26" s="6">
         <v>1221357</v>
       </c>
       <c r="J26" s="4">
-        <f>I26/$I$3</f>
+        <f t="shared" si="1"/>
         <v>6.4507701235779523E-3</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>_xll. &amp; \texttt{=_xll.RiskTriang(F9,F7,F8)} &amp;  &amp; 50,575 &amp; 0.59% &amp; 1,221,357 &amp; \textbf{0.65%}\\</v>
       </c>
     </row>
@@ -1959,18 +1989,18 @@
         <v>29191</v>
       </c>
       <c r="H27" s="4">
-        <f>G27/$G$3</f>
+        <f t="shared" si="0"/>
         <v>3.4034167547999767E-3</v>
       </c>
       <c r="I27" s="6">
         <v>1201914</v>
       </c>
       <c r="J27" s="4">
-        <f>I27/$I$3</f>
+        <f t="shared" si="1"/>
         <v>6.3480791630211898E-3</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>(' \synt{Reference} ')' &amp; \texttt{=(2*(B29))/(1+B29)} &amp;  &amp; 29,191 &amp; 0.34% &amp; 1,201,914 &amp; 0.63%\\</v>
       </c>
     </row>
@@ -1989,18 +2019,18 @@
         <v>334627</v>
       </c>
       <c r="H28" s="4">
-        <f>G28/$G$3</f>
+        <f t="shared" si="0"/>
         <v>3.9014598280581403E-2</v>
       </c>
       <c r="I28" s="6">
         <v>792299</v>
       </c>
       <c r="J28" s="4">
-        <f>I28/$I$3</f>
+        <f t="shared" si="1"/>
         <v>4.1846394773523941E-3</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'\%' &amp; \texttt{=IF(E5&gt;I8,3%,0%)} &amp;  &amp; 334,627 &amp; 3.90% &amp; 792,299 &amp; 0.42%\\</v>
       </c>
     </row>
@@ -2022,18 +2052,18 @@
         <v>13180</v>
       </c>
       <c r="H29" s="4">
-        <f>G29/$G$3</f>
+        <f t="shared" si="0"/>
         <v>1.536673386600791E-3</v>
       </c>
       <c r="I29" s="6">
         <v>324621</v>
       </c>
       <c r="J29" s="4">
-        <f>I29/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.7145318267189678E-3</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Empty argument &amp; \texttt{=DCOUNT(Lettergrades,,I80:I81)} &amp;  &amp; 13,180 &amp; 0.15% &amp; 324,621 &amp; \textbf{0.17%}\\</v>
       </c>
     </row>
@@ -2055,18 +2085,18 @@
         <v>17817</v>
       </c>
       <c r="H30" s="4">
-        <f>G30/$G$3</f>
+        <f t="shared" si="0"/>
         <v>2.0773072632068509E-3</v>
       </c>
       <c r="I30" s="7">
         <v>225621</v>
       </c>
       <c r="J30" s="8">
-        <f>I30/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.1916492934103469E-3</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Intersection &amp; \texttt{=Ending_Inventory Jan} &amp;  &amp; 17,817 &amp; 0.21% &amp; \textbf{225,621} &amp; 0.12%\\</v>
       </c>
     </row>
@@ -2091,18 +2121,18 @@
         <v>9152</v>
       </c>
       <c r="H31" s="4">
-        <f>G31/$G$3</f>
+        <f t="shared" si="0"/>
         <v>1.0670436141252231E-3</v>
       </c>
       <c r="I31" s="7">
         <v>171048</v>
       </c>
       <c r="J31" s="8">
-        <f>I31/$I$3</f>
+        <f t="shared" si="1"/>
         <v>9.0341425815528269E-4</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>FILE '!' &amp; \texttt{=[1]!today} &amp;  &amp; 9,152 &amp; 0.11% &amp; \textbf{171,048} &amp; \textbf{0.09%}\\</v>
       </c>
     </row>
@@ -2124,18 +2154,18 @@
         <v>7074</v>
       </c>
       <c r="H32" s="4">
-        <f>G32/$G$3</f>
+        <f t="shared" si="0"/>
         <v>8.2476688443201785E-4</v>
       </c>
       <c r="I32" s="7">
         <v>139851</v>
       </c>
       <c r="J32" s="8">
-        <f>I32/$I$3</f>
+        <f t="shared" si="1"/>
         <v>7.3864288046206E-4</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>UDF reference &amp; \texttt{=[1]!wbname()} &amp;  &amp; 7,074 &amp; 0.08% &amp; \textbf{139,851} &amp; 0.07%\\</v>
       </c>
     </row>
@@ -2157,18 +2187,18 @@
         <v>5140</v>
       </c>
       <c r="H33" s="4">
-        <f>G33/$G$3</f>
+        <f t="shared" si="0"/>
         <v>5.9927930251351031E-4</v>
       </c>
       <c r="I33" s="7">
         <v>137418</v>
       </c>
       <c r="J33" s="8">
-        <f>I33/$I$3</f>
+        <f t="shared" si="1"/>
         <v>7.2579264608286934E-4</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>HORIZONTAL-RANGE &amp; \texttt{=MATCH(F3,Prices!2:2,0)} &amp;  &amp; 5,140 &amp; 0.06% &amp; 137,418 &amp; \textbf{0.07%}\\</v>
       </c>
     </row>
@@ -2187,18 +2217,18 @@
         <v>1016</v>
       </c>
       <c r="H34" s="4">
-        <f>G34/$G$3</f>
+        <f t="shared" si="0"/>
         <v>1.184567648548106E-4</v>
       </c>
       <c r="I34" s="7">
         <v>54153</v>
       </c>
       <c r="J34" s="8">
-        <f>I34/$I$3</f>
+        <f t="shared" si="1"/>
         <v>2.8601674571981564E-4</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{StructureReference} &amp; \texttt{=MAX(Vertices[In-Degree])} &amp;  &amp; 1,016 &amp; 0.01% &amp; 54,153 &amp; 0.03%\\</v>
       </c>
     </row>
@@ -2220,18 +2250,18 @@
         <v>549</v>
       </c>
       <c r="H35" s="4">
-        <f>G35/$G$3</f>
+        <f t="shared" si="0"/>
         <v>6.4008625891034463E-5</v>
       </c>
       <c r="I35" s="7">
         <v>28706</v>
       </c>
       <c r="J35" s="8">
-        <f>I35/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.5161480809249768E-4</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ERROR &amp; \texttt{=IF(R14=TRUE,G19,#N/A)} &amp;  &amp; 549 &amp; 0.01% &amp; 28,706 &amp; \textbf{0.02%}\\</v>
       </c>
     </row>
@@ -2256,18 +2286,18 @@
         <v>289</v>
       </c>
       <c r="H36" s="4">
-        <f>G36/$G$3</f>
+        <f t="shared" si="0"/>
         <v>3.3694886853386084E-5</v>
       </c>
       <c r="I36" s="7">
         <v>25218</v>
       </c>
       <c r="J36" s="8">
-        <f>I36/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.3319244166643234E-4</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>MULTIPLE-SHEETS &amp; \texttt{=SUM(Sheet1:Sheet20!I29)} &amp;  &amp; 289 &amp; 0.00% &amp; \textbf{25,218} &amp; \textbf{0.01%}\\</v>
       </c>
     </row>
@@ -2292,18 +2322,18 @@
         <v>433</v>
       </c>
       <c r="H37" s="4">
-        <f>G37/$G$3</f>
+        <f t="shared" si="0"/>
         <v>5.0484034628083651E-5</v>
       </c>
       <c r="I37" s="7">
         <v>9166</v>
       </c>
       <c r="J37" s="9">
-        <f>I37/$I$3</f>
+        <f t="shared" si="1"/>
         <v>4.8411528285927463E-5</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Complex ranges &amp; \texttt{=SUM(I8:K8:M8)} &amp;  &amp; 433 &amp; 0.01% &amp; \textbf{9,166} &amp; \textbf{0.00%}\\</v>
       </c>
     </row>
@@ -2328,14 +2358,14 @@
         <v>345</v>
       </c>
       <c r="H38" s="4">
-        <f>G38/$G$3</f>
+        <f t="shared" si="0"/>
         <v>4.022399987687958E-5</v>
       </c>
       <c r="I38" s="7">
         <v>3941</v>
       </c>
       <c r="J38" s="9">
-        <f>I38/$I$3</f>
+        <f t="shared" si="1"/>
         <v>2.0814950139083585E-5</v>
       </c>
       <c r="K38" t="str">
@@ -2361,18 +2391,18 @@
         <v>3279</v>
       </c>
       <c r="H39" s="4">
-        <f>G39/$G$3</f>
+        <f t="shared" si="0"/>
         <v>3.823028857863425E-4</v>
       </c>
       <c r="I39" s="7">
         <v>3689</v>
       </c>
       <c r="J39" s="8">
-        <f>I39/$I$3</f>
+        <f t="shared" si="1"/>
         <v>1.9483976417934367E-5</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>DDECALL &amp; \texttt{=TWINDDE|RSFRec!'NGH2 NET.CHNG''} &amp;  &amp; 3,279 &amp; 0.04% &amp; \textbf{3,689} &amp; 0.00%\\</v>
       </c>
     </row>
@@ -2393,19 +2423,19 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="6">
-        <f>14+G55</f>
+        <f>14+G80</f>
         <v>32</v>
       </c>
       <c r="H40" s="4">
-        <f>G40/$G$3</f>
+        <f t="shared" si="0"/>
         <v>3.7309217277105699E-6</v>
       </c>
       <c r="I40" s="7">
-        <f>199+I55</f>
+        <f>199+I80</f>
         <v>1054</v>
       </c>
       <c r="J40" s="8">
-        <f>I40/$I$3</f>
+        <f t="shared" si="1"/>
         <v>5.5668504051241051E-6</v>
       </c>
       <c r="K40" t="str">
@@ -2431,18 +2461,18 @@
         <v>75</v>
       </c>
       <c r="H41" s="4">
-        <f>G41/$G$3</f>
+        <f t="shared" si="0"/>
         <v>8.7443477993216486E-6</v>
       </c>
       <c r="I41" s="7">
         <v>743</v>
       </c>
       <c r="J41" s="8">
-        <f>I41/$I$3</f>
+        <f t="shared" si="1"/>
         <v>3.9242598206899526E-6</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{ConstantArray} &amp; \texttt{=FVSCHEDULE(1,{0.09;0.11;0.1})} &amp;  &amp; 75 &amp; 0.00% &amp; \textbf{743} &amp; 0.00%\\</v>
       </c>
     </row>
@@ -2464,18 +2494,18 @@
         <v>32</v>
       </c>
       <c r="H42" s="4">
-        <f>G42/$G$3</f>
+        <f t="shared" si="0"/>
         <v>3.7309217277105699E-6</v>
       </c>
       <c r="I42" s="7">
         <v>672</v>
       </c>
       <c r="J42" s="8">
-        <f>I42/$I$3</f>
+        <f t="shared" si="1"/>
         <v>3.5492632563979113E-6</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>RESERVED_NAME &amp; \texttt{=C23/_xlnm.Print_Area} &amp;  &amp; 32 &amp; 0.00% &amp; \textbf{672} &amp; 0.00%\\</v>
       </c>
     </row>
@@ -2497,18 +2527,18 @@
         <v>24</v>
       </c>
       <c r="H43" s="4">
-        <f>G43/$G$3</f>
+        <f t="shared" si="0"/>
         <v>2.7981912957829274E-6</v>
       </c>
       <c r="I43" s="7">
         <v>578</v>
       </c>
       <c r="J43" s="8">
-        <f>I43/$I$3</f>
+        <f t="shared" si="1"/>
         <v>3.052788931842251E-6</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\synt{Union} &amp; \texttt{=LARGE((F38,C38),1)} &amp;  &amp; 24 &amp; 0.00% &amp; \textbf{578} &amp; 0.00%\\</v>
       </c>
     </row>
@@ -2528,14 +2558,14 @@
         <v>4530</v>
       </c>
       <c r="H50" s="4">
-        <f>G50/$G$3</f>
+        <f t="shared" ref="H50:H56" si="3">G50/$G$3</f>
         <v>5.281586070790276E-4</v>
       </c>
       <c r="I50" s="6">
         <v>549846</v>
       </c>
       <c r="J50" s="4">
-        <f>I50/$I$3</f>
+        <f t="shared" ref="J50:J56" si="4">I50/$I$3</f>
         <v>2.9040895899960805E-3</v>
       </c>
     </row>
@@ -2555,14 +2585,14 @@
         <v>36565</v>
       </c>
       <c r="H51" s="4">
-        <f>G51/$G$3</f>
+        <f t="shared" si="3"/>
         <v>4.2631610304292812E-3</v>
       </c>
       <c r="I51" s="6">
         <v>1302505</v>
       </c>
       <c r="J51" s="4">
-        <f>I51/$I$3</f>
+        <f t="shared" si="4"/>
         <v>6.8793647883550026E-3</v>
       </c>
     </row>
@@ -2579,14 +2609,14 @@
         <v>681838</v>
       </c>
       <c r="H52" s="4">
-        <f>G52/$G$3</f>
+        <f t="shared" si="3"/>
         <v>7.9496381530584984E-2</v>
       </c>
       <c r="I52" s="6">
         <v>27648922</v>
       </c>
       <c r="J52" s="4">
-        <f>I52/$I$3</f>
+        <f t="shared" si="4"/>
         <v>0.14603170079406527</v>
       </c>
     </row>
@@ -2603,14 +2633,14 @@
         <v>985</v>
       </c>
       <c r="H53" s="4">
-        <f>G53/$G$3</f>
+        <f t="shared" si="3"/>
         <v>1.1484243443109098E-4</v>
       </c>
       <c r="I53" s="6">
         <v>107129</v>
       </c>
       <c r="J53" s="4">
-        <f>I53/$I$3</f>
+        <f t="shared" si="4"/>
         <v>5.6581699909918426E-4</v>
       </c>
     </row>
@@ -2630,14 +2660,14 @@
         <v>8760</v>
       </c>
       <c r="H54" s="4">
-        <f>G54/$G$3</f>
+        <f t="shared" si="3"/>
         <v>1.0213398229607686E-3</v>
       </c>
       <c r="I54" s="6">
         <v>186925</v>
       </c>
       <c r="J54" s="4">
-        <f>I54/$I$3</f>
+        <f t="shared" si="4"/>
         <v>9.8727088422943397E-4</v>
       </c>
     </row>
@@ -2645,54 +2675,18 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="6">
-        <v>18</v>
-      </c>
-      <c r="H55" s="4">
-        <f>G55/$G$3</f>
-        <v>2.0986434718371954E-6</v>
-      </c>
-      <c r="I55" s="6">
-        <v>855</v>
-      </c>
-      <c r="J55" s="4">
-        <f>I55/$I$3</f>
-        <v>4.5158036967562716E-6</v>
-      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-      <c r="D56" t="s">
-        <v>37</v>
-      </c>
-      <c r="G56" s="6">
-        <v>4</v>
-      </c>
-      <c r="H56" s="4">
-        <f>G56/$G$3</f>
-        <v>4.6636521596382123E-7</v>
-      </c>
-      <c r="I56" s="6">
-        <v>257</v>
-      </c>
-      <c r="J56" s="4">
-        <f>I56/$I$3</f>
-        <v>1.3573819299021774E-6</v>
-      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -2700,7 +2694,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -2714,11 +2708,11 @@
         <v>11052382</v>
       </c>
       <c r="H71" s="4">
-        <f t="shared" ref="H66:H74" si="1">B71/D71</f>
+        <f t="shared" ref="H71:H74" si="5">B71/D71</f>
         <v>1.6275677044097825E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -2732,11 +2726,11 @@
         <v>21160683</v>
       </c>
       <c r="H72" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.164391385665576E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -2750,11 +2744,11 @@
         <v>1260846</v>
       </c>
       <c r="H73" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.5751328869663703E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>92</v>
       </c>
@@ -2768,14 +2762,120 @@
         <v>155861157</v>
       </c>
       <c r="H74" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.7776003228309156E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B76" s="4">
         <f>B71/SUM(B71:B74)</f>
         <v>0.79728837297946553</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D78" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G78" s="6">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="6">
+        <v>18</v>
+      </c>
+      <c r="H80" s="4">
+        <f>G80/$G$3</f>
+        <v>2.0986434718371954E-6</v>
+      </c>
+      <c r="I80" s="6">
+        <v>855</v>
+      </c>
+      <c r="J80" s="4">
+        <f>I80/$I$3</f>
+        <v>4.5158036967562716E-6</v>
+      </c>
+    </row>
+    <row r="81" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>37</v>
+      </c>
+      <c r="G81" s="6">
+        <v>4</v>
+      </c>
+      <c r="H81" s="4">
+        <f>G81/$G$3</f>
+        <v>4.6636521596382123E-7</v>
+      </c>
+      <c r="I81" s="6">
+        <v>257</v>
+      </c>
+      <c r="J81" s="4">
+        <f>I81/$I$3</f>
+        <v>1.3573819299021774E-6</v>
+      </c>
+    </row>
+    <row r="82" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>94</v>
+      </c>
+      <c r="G82" s="6">
+        <v>1</v>
+      </c>
+      <c r="I82" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>95</v>
+      </c>
+      <c r="G83" s="6">
+        <v>3</v>
+      </c>
+      <c r="I83" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>96</v>
+      </c>
+      <c r="G84" s="6">
+        <v>65</v>
+      </c>
+      <c r="I84" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="85" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>97</v>
+      </c>
+      <c r="G85" s="6">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="86" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="G91" s="6">
+        <f>SUM(G80:G87)</f>
+        <v>930</v>
+      </c>
+    </row>
+    <row r="96" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="G96" s="6">
+        <f>G91+457</f>
+        <v>1387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>